<commit_message>
Interface has been updated to add nitrous oxide as a gas and irrigation has been updated to add flooding intput files have been updated
</commit_message>
<xml_diff>
--- a/Example input/CO2_Respiration_CaseStudy2/CaseStudy2.xlsx
+++ b/Example input/CO2_Respiration_CaseStudy2/CaseStudy2.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B077EC3-AE21-4EAC-A41B-D0D4DA629AD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D991FF04-F0CE-4770-91EB-509B51A322D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25092" yWindow="2496" windowWidth="17280" windowHeight="9540" tabRatio="626" firstSheet="6" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20625" yWindow="2115" windowWidth="17250" windowHeight="11820" tabRatio="626" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="16" r:id="rId1"/>
@@ -29,7 +29,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">Soil!$A$1:$A$6</definedName>
-    <definedName name="Description">Description!$A$1:$T$1</definedName>
+    <definedName name="Description">Description!$A$1:$U$1</definedName>
     <definedName name="Fertilization">Fertilization!$A$1:$F$1</definedName>
     <definedName name="GridRatio">GridRatio!$A$1:$J$1</definedName>
     <definedName name="GridX">#REF!</definedName>
@@ -39,7 +39,7 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="16" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="4" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
-    <definedName name="Soil">Soil!$A$1:$AS$1</definedName>
+    <definedName name="Soil">Soil!$A$1:$AT$1</definedName>
     <definedName name="Time">Time!$A$1:$K$1</definedName>
     <definedName name="Weather">Weather!$A$1:$E$1</definedName>
   </definedNames>
@@ -57,8 +57,119 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{0C2168C7-E186-4C4F-B2BC-AEF8922FF8CE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+rate for sprinkler or ponding when ponded as a flow of water into the field
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{B23D1978-7DA7-4211-A55B-521BEDD1853A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+the target ponded depth for flow infil or constant depth</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{BC3E0621-CC7E-411E-8A5F-0169324FF37E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+type can be:
+flood_H flooding as a depth of water
+flood_R flooding as a rate of water input
+sprinkler
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{57D50D64-4586-4D36-803E-9D3FB94522DA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+hour of day 0-23</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="299">
   <si>
     <t>Date</t>
   </si>
@@ -889,6 +1000,72 @@
   </si>
   <si>
     <t>amount (mm/day)</t>
+  </si>
+  <si>
+    <t>Gas_N2O</t>
+  </si>
+  <si>
+    <t>GasN2ODefault</t>
+  </si>
+  <si>
+    <t>N2O(ppm)</t>
+  </si>
+  <si>
+    <t>date_start</t>
+  </si>
+  <si>
+    <t>date_end</t>
+  </si>
+  <si>
+    <t>Depth (mm)</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>start_hour</t>
+  </si>
+  <si>
+    <t>end_hour</t>
+  </si>
+  <si>
+    <t>there are 3 types of irrigation</t>
+  </si>
+  <si>
+    <t>flood_H</t>
+  </si>
+  <si>
+    <t>flooding by applying ponded water head</t>
+  </si>
+  <si>
+    <t>flood_R</t>
+  </si>
+  <si>
+    <t>flooding by applying a rate of water application over time</t>
+  </si>
+  <si>
+    <t>Sprinkler</t>
+  </si>
+  <si>
+    <t>overhead sprinkler</t>
+  </si>
+  <si>
+    <t>sprinkler</t>
+  </si>
+  <si>
+    <t>enter date_start and date_end, depth start_hour and end_hour and depth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flood_R </t>
+  </si>
+  <si>
+    <t>enter date_start and date_end, depth start_hour and end_hour and amount</t>
+  </si>
+  <si>
+    <t>enter date start and amount</t>
+  </si>
+  <si>
+    <t>example</t>
   </si>
 </sst>
 </file>
@@ -900,7 +1077,7 @@
     <numFmt numFmtId="165" formatCode="h:mm;@"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -940,6 +1117,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1419,12 +1609,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:X3"/>
+  <dimension ref="A1:Y3"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
+      <selection pane="bottomLeft" activeCell="S1" sqref="S1:S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1444,12 +1634,12 @@
     <col min="15" max="15" width="21.33203125" customWidth="1"/>
     <col min="16" max="16" width="16.33203125" customWidth="1"/>
     <col min="17" max="17" width="24.6640625" customWidth="1"/>
-    <col min="18" max="18" width="24.88671875" customWidth="1"/>
-    <col min="19" max="19" width="16.109375" customWidth="1"/>
-    <col min="20" max="20" width="15.88671875" customWidth="1"/>
+    <col min="18" max="19" width="24.88671875" customWidth="1"/>
+    <col min="20" max="20" width="16.109375" customWidth="1"/>
+    <col min="21" max="21" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1505,22 +1695,25 @@
         <v>220</v>
       </c>
       <c r="S1" t="s">
+        <v>277</v>
+      </c>
+      <c r="T1" t="s">
         <v>224</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>219</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>149</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>152</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="21" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" s="21" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>243</v>
       </c>
@@ -1577,23 +1770,26 @@
       <c r="R2" s="21" t="s">
         <v>221</v>
       </c>
-      <c r="S2" s="21" t="s">
+      <c r="S2" t="s">
+        <v>278</v>
+      </c>
+      <c r="T2" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="T2" s="21" t="s">
+      <c r="U2" s="21" t="s">
         <v>218</v>
       </c>
-      <c r="U2" s="21" t="s">
+      <c r="V2" s="21" t="s">
         <v>240</v>
       </c>
-      <c r="W2" s="21" t="s">
+      <c r="X2" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="X2" s="21">
+      <c r="Y2" s="21">
         <v>2004</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J3" s="20"/>
     </row>
   </sheetData>
@@ -1660,10 +1856,10 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92F41622-738B-41A7-B4B2-43DDC1442E35}">
   <sheetPr codeName="Sheet18"/>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M41" sqref="M41"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1851,6 +2047,20 @@
       </c>
       <c r="D13">
         <v>15400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>278</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>0.65</v>
+      </c>
+      <c r="D14">
+        <v>12355.2</v>
       </c>
     </row>
   </sheetData>
@@ -1996,11 +2206,11 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:AS6"/>
+  <dimension ref="A1:AT6"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A2" sqref="A2:XFD15"/>
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2008,12 +2218,12 @@
     <col min="1" max="1" width="43.6640625" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="4" max="31" width="13" customWidth="1"/>
-    <col min="32" max="32" width="13" style="22" customWidth="1"/>
-    <col min="33" max="45" width="13" customWidth="1"/>
+    <col min="4" max="32" width="13" customWidth="1"/>
+    <col min="33" max="33" width="13" style="22" customWidth="1"/>
+    <col min="34" max="46" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>165</v>
       </c>
@@ -2062,95 +2272,98 @@
       <c r="P1" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="R1" t="s">
         <v>126</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>127</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>128</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>10</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>87</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>88</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>93</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>94</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>95</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>96</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>97</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>98</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>99</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>100</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>101</v>
       </c>
-      <c r="AF1" s="22" t="s">
+      <c r="AG1" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>66</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>67</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>68</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>58</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>69</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>70</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>59</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>60</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>61</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>62</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>63</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>64</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:45" s="27" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:46" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
         <v>249</v>
       </c>
@@ -2199,27 +2412,27 @@
       <c r="P2" s="27">
         <v>206000</v>
       </c>
-      <c r="Q2" s="27">
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2" s="27">
         <v>32</v>
       </c>
-      <c r="R2" s="27">
+      <c r="S2" s="27">
         <v>51</v>
       </c>
-      <c r="S2" s="27">
-        <f t="shared" ref="S2:S6" si="0">100-Q2-R2</f>
+      <c r="T2" s="27">
+        <f t="shared" ref="T2:T6" si="0">100-R2-S2</f>
         <v>17</v>
       </c>
-      <c r="T2" s="27">
+      <c r="U2" s="27">
         <v>1.04</v>
       </c>
-      <c r="U2" s="27">
+      <c r="V2" s="27">
         <v>0.37</v>
       </c>
-      <c r="V2" s="27">
+      <c r="W2" s="27">
         <v>0.22</v>
-      </c>
-      <c r="W2" s="27">
-        <v>-1</v>
       </c>
       <c r="X2" s="27">
         <v>-1</v>
@@ -2237,58 +2450,61 @@
         <v>-1</v>
       </c>
       <c r="AC2" s="27">
+        <v>-1</v>
+      </c>
+      <c r="AD2" s="27">
         <v>11</v>
       </c>
-      <c r="AD2" s="27">
+      <c r="AE2" s="27">
         <v>10</v>
       </c>
-      <c r="AE2" s="27">
+      <c r="AF2" s="27">
         <v>-1</v>
       </c>
-      <c r="AF2" s="28">
+      <c r="AG2" s="28">
         <v>6.9999999999999994E-5</v>
       </c>
-      <c r="AG2" s="27">
+      <c r="AH2" s="27">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="AH2" s="27">
+      <c r="AI2" s="27">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AI2" s="27">
+      <c r="AJ2" s="27">
         <v>0.2</v>
       </c>
-      <c r="AJ2" s="27">
+      <c r="AK2" s="27">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="AK2" s="27">
+      <c r="AL2" s="27">
         <v>0.6</v>
       </c>
-      <c r="AL2" s="27">
+      <c r="AM2" s="27">
         <v>0.2</v>
       </c>
-      <c r="AM2" s="27">
+      <c r="AN2" s="27">
         <v>10</v>
       </c>
-      <c r="AN2" s="27">
+      <c r="AO2" s="27">
         <v>50</v>
       </c>
-      <c r="AO2" s="27">
+      <c r="AP2" s="27">
         <v>10</v>
       </c>
-      <c r="AP2" s="27">
+      <c r="AQ2" s="27">
         <v>0.1</v>
       </c>
-      <c r="AQ2" s="27">
+      <c r="AR2" s="27">
         <v>8</v>
       </c>
-      <c r="AR2" s="27">
+      <c r="AS2" s="27">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="AS2" s="27">
+      <c r="AT2" s="27">
         <v>0.38600000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>249</v>
       </c>
@@ -2338,26 +2554,26 @@
         <v>206000</v>
       </c>
       <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
         <v>29</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>53</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>1.37</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <v>0.37</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>0.22</v>
-      </c>
-      <c r="W3">
-        <v>-1</v>
       </c>
       <c r="X3">
         <v>-1</v>
@@ -2375,58 +2591,61 @@
         <v>-1</v>
       </c>
       <c r="AC3">
+        <v>-1</v>
+      </c>
+      <c r="AD3">
         <v>11</v>
       </c>
-      <c r="AD3">
+      <c r="AE3">
         <v>10</v>
       </c>
-      <c r="AE3">
+      <c r="AF3">
         <v>-1</v>
       </c>
-      <c r="AF3" s="22">
+      <c r="AG3" s="22">
         <v>6.9999999999999994E-5</v>
       </c>
-      <c r="AG3" s="27">
+      <c r="AH3" s="27">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="AH3">
+      <c r="AI3">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AI3">
+      <c r="AJ3">
         <v>0.2</v>
       </c>
-      <c r="AJ3">
+      <c r="AK3">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="AK3">
+      <c r="AL3">
         <v>0.6</v>
       </c>
-      <c r="AL3">
+      <c r="AM3">
         <v>0.2</v>
       </c>
-      <c r="AM3">
+      <c r="AN3">
         <v>10</v>
       </c>
-      <c r="AN3">
+      <c r="AO3">
         <v>50</v>
       </c>
-      <c r="AO3">
+      <c r="AP3">
         <v>10</v>
       </c>
-      <c r="AP3">
+      <c r="AQ3">
         <v>0.1</v>
       </c>
-      <c r="AQ3">
+      <c r="AR3">
         <v>8</v>
       </c>
-      <c r="AR3">
+      <c r="AS3">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="AS3">
+      <c r="AT3">
         <v>0.38600000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>249</v>
       </c>
@@ -2476,26 +2695,26 @@
         <v>206000</v>
       </c>
       <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
         <v>28</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>52</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>1.51</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>0.37</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>0.22</v>
-      </c>
-      <c r="W4">
-        <v>-1</v>
       </c>
       <c r="X4">
         <v>-1</v>
@@ -2513,58 +2732,61 @@
         <v>-1</v>
       </c>
       <c r="AC4">
+        <v>-1</v>
+      </c>
+      <c r="AD4">
         <v>11</v>
       </c>
-      <c r="AD4">
+      <c r="AE4">
         <v>10</v>
       </c>
-      <c r="AE4">
+      <c r="AF4">
         <v>-1</v>
       </c>
-      <c r="AF4" s="22">
+      <c r="AG4" s="22">
         <v>6.9999999999999994E-5</v>
       </c>
-      <c r="AG4" s="27">
+      <c r="AH4" s="27">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="AH4">
+      <c r="AI4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AI4">
+      <c r="AJ4">
         <v>0.2</v>
       </c>
-      <c r="AJ4">
+      <c r="AK4">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="AK4">
+      <c r="AL4">
         <v>0.6</v>
       </c>
-      <c r="AL4">
+      <c r="AM4">
         <v>0.2</v>
       </c>
-      <c r="AM4">
+      <c r="AN4">
         <v>10</v>
       </c>
-      <c r="AN4">
+      <c r="AO4">
         <v>50</v>
       </c>
-      <c r="AO4">
+      <c r="AP4">
         <v>10</v>
       </c>
-      <c r="AP4">
+      <c r="AQ4">
         <v>0.1</v>
       </c>
-      <c r="AQ4">
+      <c r="AR4">
         <v>8</v>
       </c>
-      <c r="AR4">
+      <c r="AS4">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="AS4">
+      <c r="AT4">
         <v>0.38600000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>249</v>
       </c>
@@ -2614,26 +2836,26 @@
         <v>206000</v>
       </c>
       <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
         <v>29</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>51</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>1.58</v>
       </c>
-      <c r="U5">
+      <c r="V5">
         <v>0.37</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>0.22</v>
-      </c>
-      <c r="W5">
-        <v>-1</v>
       </c>
       <c r="X5">
         <v>-1</v>
@@ -2651,58 +2873,61 @@
         <v>-1</v>
       </c>
       <c r="AC5">
+        <v>-1</v>
+      </c>
+      <c r="AD5">
         <v>11</v>
       </c>
-      <c r="AD5">
+      <c r="AE5">
         <v>10</v>
       </c>
-      <c r="AE5">
+      <c r="AF5">
         <v>-1</v>
       </c>
-      <c r="AF5" s="22">
+      <c r="AG5" s="22">
         <v>6.9999999999999994E-5</v>
       </c>
-      <c r="AG5" s="27">
+      <c r="AH5" s="27">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="AH5">
+      <c r="AI5">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AI5">
+      <c r="AJ5">
         <v>0.2</v>
       </c>
-      <c r="AJ5">
+      <c r="AK5">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="AK5">
+      <c r="AL5">
         <v>0.6</v>
       </c>
-      <c r="AL5">
+      <c r="AM5">
         <v>0.2</v>
       </c>
-      <c r="AM5">
+      <c r="AN5">
         <v>10</v>
       </c>
-      <c r="AN5">
+      <c r="AO5">
         <v>50</v>
       </c>
-      <c r="AO5">
+      <c r="AP5">
         <v>10</v>
       </c>
-      <c r="AP5">
+      <c r="AQ5">
         <v>0.1</v>
       </c>
-      <c r="AQ5">
+      <c r="AR5">
         <v>8</v>
       </c>
-      <c r="AR5">
+      <c r="AS5">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="AS5">
+      <c r="AT5">
         <v>0.38600000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>249</v>
       </c>
@@ -2752,26 +2977,26 @@
         <v>206000</v>
       </c>
       <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
         <v>33</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>48</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>1.58</v>
       </c>
-      <c r="U6">
+      <c r="V6">
         <v>0.37</v>
       </c>
-      <c r="V6">
+      <c r="W6">
         <v>0.22</v>
-      </c>
-      <c r="W6">
-        <v>-1</v>
       </c>
       <c r="X6">
         <v>-1</v>
@@ -2789,54 +3014,57 @@
         <v>-1</v>
       </c>
       <c r="AC6">
+        <v>-1</v>
+      </c>
+      <c r="AD6">
         <v>11</v>
       </c>
-      <c r="AD6">
+      <c r="AE6">
         <v>10</v>
       </c>
-      <c r="AE6">
+      <c r="AF6">
         <v>-1</v>
       </c>
-      <c r="AF6" s="22">
+      <c r="AG6" s="22">
         <v>6.9999999999999994E-5</v>
       </c>
-      <c r="AG6" s="27">
+      <c r="AH6" s="27">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="AH6">
+      <c r="AI6">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AI6">
+      <c r="AJ6">
         <v>0.2</v>
       </c>
-      <c r="AJ6">
+      <c r="AK6">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="AK6">
+      <c r="AL6">
         <v>0.6</v>
       </c>
-      <c r="AL6">
+      <c r="AM6">
         <v>0.2</v>
       </c>
-      <c r="AM6">
+      <c r="AN6">
         <v>10</v>
       </c>
-      <c r="AN6">
+      <c r="AO6">
         <v>50</v>
       </c>
-      <c r="AO6">
+      <c r="AP6">
         <v>10</v>
       </c>
-      <c r="AP6">
+      <c r="AQ6">
         <v>0.1</v>
       </c>
-      <c r="AQ6">
+      <c r="AR6">
         <v>8</v>
       </c>
-      <c r="AR6">
+      <c r="AS6">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="AS6">
+      <c r="AT6">
         <v>0.38600000000000001</v>
       </c>
     </row>
@@ -3887,7 +4115,7 @@
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -4965,12 +5193,12 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:C212"/>
+  <dimension ref="A1:M212"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4980,60 +5208,166 @@
     <col min="3" max="3" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>167</v>
       </c>
       <c r="B1" t="s">
-        <v>146</v>
+        <v>280</v>
       </c>
       <c r="C1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D1" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B2" s="6"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B3" s="6"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="6"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="6"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B6" s="6"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B7" s="6"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B8" s="6"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>282</v>
+      </c>
+      <c r="F1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G1" t="s">
+        <v>284</v>
+      </c>
+      <c r="H1" t="s">
+        <v>285</v>
+      </c>
+      <c r="L1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B2" s="1">
+        <v>38842</v>
+      </c>
+      <c r="C2" s="1">
+        <v>38847</v>
+      </c>
+      <c r="E2">
+        <v>50</v>
+      </c>
+      <c r="F2" t="s">
+        <v>287</v>
+      </c>
+      <c r="G2">
+        <v>12</v>
+      </c>
+      <c r="H2">
+        <v>18</v>
+      </c>
+      <c r="L2" t="s">
+        <v>287</v>
+      </c>
+      <c r="M2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>298</v>
+      </c>
+      <c r="B3" s="1">
+        <v>38863</v>
+      </c>
+      <c r="C3" s="1">
+        <v>38869</v>
+      </c>
+      <c r="D3">
+        <v>270</v>
+      </c>
+      <c r="E3">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
+        <v>289</v>
+      </c>
+      <c r="G3">
+        <v>8</v>
+      </c>
+      <c r="H3">
+        <v>18</v>
+      </c>
+      <c r="L3" t="s">
+        <v>289</v>
+      </c>
+      <c r="M3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>298</v>
+      </c>
+      <c r="B4" s="1">
+        <v>38504</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4">
+        <v>200</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>293</v>
+      </c>
+      <c r="L4" t="s">
+        <v>291</v>
+      </c>
+      <c r="M4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L6" t="s">
+        <v>287</v>
+      </c>
+      <c r="M6" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L7" t="s">
+        <v>295</v>
+      </c>
+      <c r="M7" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L8" t="s">
+        <v>293</v>
+      </c>
+      <c r="M8" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B9" s="6"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B10" s="6"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11" s="6"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B12" s="6"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B13" s="6"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B14" s="6"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B15" s="6"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B16" s="6"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
@@ -5627,6 +5961,7 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5956,15 +6291,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010086EABF47CD1113448A96A17F6C8D13F9" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c68283fca48dae9b1add248de89d15c2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a5f42ec3-4ee2-45fc-8d77-288bf2f0f986" xmlns:ns3="73fb875a-8af9-4255-b008-0995492d31cd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40d2b883f32ec076906f2da59f0ebb5f" ns2:_="" ns3:_="">
     <xsd:import namespace="a5f42ec3-4ee2-45fc-8d77-288bf2f0f986"/>
@@ -6153,15 +6479,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA6A39AF-B78F-46A4-B576-74869F9A9581}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDA73D10-6EB9-46B2-AEC6-EC67F487A9BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6178,4 +6505,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA6A39AF-B78F-46A4-B576-74869F9A9581}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>